<commit_message>
Cancel button now appears even if the reservation group is not confirmed. Closes #156
</commit_message>
<xml_diff>
--- a/public/spreadsheets/exemplo_reserva_em_lote.xlsx
+++ b/public/spreadsheets/exemplo_reserva_em_lote.xlsx
@@ -449,7 +449,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -460,7 +460,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -522,10 +522,10 @@
         <v>12</v>
       </c>
       <c r="F2" s="1">
-        <v>41932</v>
+        <v>42297</v>
       </c>
       <c r="G2" s="1">
-        <v>42190</v>
+        <v>42556</v>
       </c>
       <c r="H2">
         <v>23</v>
@@ -539,10 +539,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="F3" s="1">
-        <v>41932</v>
+        <v>42297</v>
       </c>
       <c r="G3" s="1">
-        <v>42190</v>
+        <v>42556</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -568,10 +568,10 @@
         <v>12</v>
       </c>
       <c r="F4" s="1">
-        <v>41932</v>
+        <v>42297</v>
       </c>
       <c r="G4" s="1">
-        <v>42190</v>
+        <v>42556</v>
       </c>
       <c r="H4">
         <v>24</v>
@@ -585,10 +585,10 @@
     </row>
     <row r="5" spans="1:10">
       <c r="F5" s="1">
-        <v>41932</v>
+        <v>42297</v>
       </c>
       <c r="G5" s="1">
-        <v>42190</v>
+        <v>42556</v>
       </c>
       <c r="H5">
         <v>5</v>

</xml_diff>